<commit_message>
newest files for fermentation rate data
</commit_message>
<xml_diff>
--- a/fermini_leale.xlsx
+++ b/fermini_leale.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/alanna_leale_wur_nl/Documents/2023_montpellier/experiments/weights/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/alanna_leale_wur_nl/Documents/2023_montpellier/experiments/data/weights/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8_{8AA6E514-4721-3F45-A096-1DF4F0800EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8_{6412871A-E87F-E648-83A3-BEC0D54A3D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33320" yWindow="500" windowWidth="29620" windowHeight="19400" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="4657" uniqueCount="2113">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="4658" uniqueCount="2114">
   <si>
     <t>Fermentation n° 4247</t>
   </si>
@@ -6383,6 +6383,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>richness</t>
   </si>
 </sst>
 </file>
@@ -31463,15 +31466,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A009CA21-BF59-6542-B22D-5CCD8DF26820}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="18" t="s">
         <v>67</v>
       </c>
@@ -31493,8 +31496,11 @@
       <c r="G1" s="18" t="s">
         <v>2110</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="18" t="s">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="16" t="s">
         <v>36</v>
       </c>
@@ -31516,8 +31522,11 @@
       <c r="G2" s="18" t="s">
         <v>2112</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="16" t="s">
         <v>109</v>
       </c>
@@ -31539,8 +31548,11 @@
       <c r="G3" s="18" t="s">
         <v>2112</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="16" t="s">
         <v>155</v>
       </c>
@@ -31562,8 +31574,11 @@
       <c r="G4" s="18" t="s">
         <v>2112</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="16" t="s">
         <v>199</v>
       </c>
@@ -31585,8 +31600,11 @@
       <c r="G5" s="18" t="s">
         <v>2112</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="16" t="s">
         <v>238</v>
       </c>
@@ -31608,8 +31626,11 @@
       <c r="G6" s="23" t="s">
         <v>2111</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="16" t="s">
         <v>277</v>
       </c>
@@ -31631,8 +31652,11 @@
       <c r="G7" s="18" t="s">
         <v>2112</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="16" t="s">
         <v>313</v>
       </c>
@@ -31654,8 +31678,11 @@
       <c r="G8" s="23" t="s">
         <v>2111</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="16" t="s">
         <v>347</v>
       </c>
@@ -31677,8 +31704,11 @@
       <c r="G9" s="23" t="s">
         <v>2111</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="16" t="s">
         <v>382</v>
       </c>
@@ -31700,8 +31730,11 @@
       <c r="G10" s="23" t="s">
         <v>2111</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="16" t="s">
         <v>417</v>
       </c>
@@ -31723,8 +31756,11 @@
       <c r="G11" s="18" t="s">
         <v>2112</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="16" t="s">
         <v>452</v>
       </c>
@@ -31746,8 +31782,11 @@
       <c r="G12" s="18" t="s">
         <v>2112</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="16" t="s">
         <v>486</v>
       </c>
@@ -31769,8 +31808,11 @@
       <c r="G13" s="18" t="s">
         <v>2112</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="16" t="s">
         <v>522</v>
       </c>
@@ -31792,8 +31834,11 @@
       <c r="G14" s="23" t="s">
         <v>2111</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="16" t="s">
         <v>557</v>
       </c>
@@ -31815,8 +31860,11 @@
       <c r="G15" s="18" t="s">
         <v>2112</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="16" t="s">
         <v>594</v>
       </c>
@@ -31838,8 +31886,11 @@
       <c r="G16" s="23" t="s">
         <v>2111</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="16" t="s">
         <v>630</v>
       </c>
@@ -31861,8 +31912,11 @@
       <c r="G17" s="23" t="s">
         <v>2111</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="16" t="s">
         <v>667</v>
       </c>
@@ -31883,6 +31937,9 @@
       </c>
       <c r="G18" s="23" t="s">
         <v>2111</v>
+      </c>
+      <c r="H18" s="18">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>